<commit_message>
Ficha de dados para preenchimento no BD
</commit_message>
<xml_diff>
--- a/Ficha-de-Dados-Iglu.xlsx
+++ b/Ficha-de-Dados-Iglu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Fatec\6\LAB-ES\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74FE924-4E7B-4C25-92DC-B6A7656DD62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6713E7-88E8-47C5-B4A0-868F65D35C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{5D62AE46-FB4E-4EA0-91C3-D284FB033502}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D62AE46-FB4E-4EA0-91C3-D284FB033502}"/>
   </bookViews>
   <sheets>
     <sheet name="Estoque de produtos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="187">
   <si>
     <t>Nome do produto</t>
   </si>
@@ -86,12 +86,6 @@
     <t>Pote</t>
   </si>
   <si>
-    <t>Picolé sabor chocolate ao leite envolvido por sorvete de creme e coberto com casquinha de chocolate branco. 72ml</t>
-  </si>
-  <si>
-    <t>Sorvete de baunilha com lascas crocantes de chocolate branco Magnum. 297g/440ml</t>
-  </si>
-  <si>
     <t>L24112022</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>L30122022</t>
   </si>
   <si>
-    <t>Sorvete colorido de morango com chatilly. 800ml</t>
-  </si>
-  <si>
     <t>Gelato sabor Pistache</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>BACIO Di LATTE</t>
   </si>
   <si>
-    <t>Gelato italiano à base de leite, pistaches e creme de leite. 490ml</t>
-  </si>
-  <si>
     <t>Funcionários</t>
   </si>
   <si>
@@ -386,9 +374,6 @@
     <t>Nestlé</t>
   </si>
   <si>
-    <t>Sorvete Napolitano Trio Moça. 1,5L</t>
-  </si>
-  <si>
     <t>Sorvete Flocos Nobrelli</t>
   </si>
   <si>
@@ -398,9 +383,6 @@
     <t>Nobrelli</t>
   </si>
   <si>
-    <t>Sorvete de flocos Nobrelli. 1,5L</t>
-  </si>
-  <si>
     <t>contato.sorvetes@nobrelli.com.br</t>
   </si>
   <si>
@@ -431,9 +413,6 @@
     <t>Lacta</t>
   </si>
   <si>
-    <t>Sorvete Sonho de Valsa edição especial. 1L</t>
-  </si>
-  <si>
     <t>contato.sorvetes.nestle@nestle.com.br</t>
   </si>
   <si>
@@ -518,9 +497,6 @@
     <t>L29112022</t>
   </si>
   <si>
-    <t>Casquinha/cone para sorvetes. 450g cada</t>
-  </si>
-  <si>
     <t>Sorvete de casquinha Napolitano</t>
   </si>
   <si>
@@ -551,13 +527,79 @@
     <t>Marvi Embalagens</t>
   </si>
   <si>
-    <t>Copo plástico Copaza 550ml</t>
-  </si>
-  <si>
     <t>Susan Melo</t>
   </si>
   <si>
     <t>Sundae de sonho de valsa</t>
+  </si>
+  <si>
+    <t>72ml</t>
+  </si>
+  <si>
+    <t>800ml</t>
+  </si>
+  <si>
+    <t>490ml</t>
+  </si>
+  <si>
+    <t>1,5L</t>
+  </si>
+  <si>
+    <t>1L</t>
+  </si>
+  <si>
+    <t>550ml</t>
+  </si>
+  <si>
+    <t>440ml</t>
+  </si>
+  <si>
+    <t>450g</t>
+  </si>
+  <si>
+    <t>Copo plástico Copaza</t>
+  </si>
+  <si>
+    <t>Casquinha/cone para sorvetes.</t>
+  </si>
+  <si>
+    <t>Sorvete Sonho de Valsa edição especial.</t>
+  </si>
+  <si>
+    <t>Picolé sabor chocolate ao leite envolvido por sorvete de creme e coberto com casquinha de chocolate branco.</t>
+  </si>
+  <si>
+    <t>Sorvete de baunilha com lascas crocantes de chocolate branco Magnum.</t>
+  </si>
+  <si>
+    <t>Sorvete colorido de morango com chatilly.</t>
+  </si>
+  <si>
+    <t>Gelato italiano à base de leite, pistaches e creme de leite.</t>
+  </si>
+  <si>
+    <t>Sorvete Napolitano Trio Moça.</t>
+  </si>
+  <si>
+    <t>Sorvete de flocos Nobrelli.</t>
+  </si>
+  <si>
+    <t>85.151.504/0001-65</t>
+  </si>
+  <si>
+    <t>(48) 3461-3000</t>
+  </si>
+  <si>
+    <t>Ana Luiza Zanatta</t>
+  </si>
+  <si>
+    <t>analuiza91@copaza.com.br</t>
+  </si>
+  <si>
+    <t>(48) 2134-5657</t>
+  </si>
+  <si>
+    <t>Peso medida</t>
   </si>
 </sst>
 </file>
@@ -751,6 +793,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,9 +803,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1108,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E0B53C-A798-4C93-B956-3BC70144FA2F}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1125,64 +1167,69 @@
     <col min="9" max="9" width="15.109375" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="11" max="11" width="26.21875" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
-    </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="L2" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -1203,21 +1250,24 @@
         <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -1238,21 +1288,24 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -1273,21 +1326,24 @@
         <v>29.99</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -1308,21 +1364,24 @@
         <v>41.99</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -1343,21 +1402,24 @@
         <v>23.9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -1378,21 +1440,24 @@
         <v>22.99</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1413,24 +1478,27 @@
         <v>32.94</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D10" s="6">
         <v>44813</v>
@@ -1448,24 +1516,27 @@
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D11" s="6">
         <v>44765</v>
@@ -1483,18 +1554,21 @@
         <v>3.5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1507,7 +1581,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,41 +1596,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1567,22 +1641,22 @@
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1590,25 +1664,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1616,25 +1690,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>124</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1642,25 +1716,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1668,25 +1742,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="F7" s="11" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1694,25 +1768,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1720,16 +1794,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
+        <v>156</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1750,9 +1834,10 @@
     <hyperlink ref="C8" r:id="rId11" xr:uid="{5637C27D-5A99-49B4-9E8F-22AE6C9C8D25}"/>
     <hyperlink ref="G8" r:id="rId12" xr:uid="{974F9725-870A-4C9E-B594-97A855877F72}"/>
     <hyperlink ref="C9" r:id="rId13" xr:uid="{86431905-E9D0-4748-A544-7C3867227F78}"/>
+    <hyperlink ref="G9" r:id="rId14" xr:uid="{D26AAC77-938B-41CF-9667-6304C8243C0A}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -1783,69 +1868,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="A1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="N2" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1853,46 +1938,46 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="6">
         <v>32878</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I3" s="1">
         <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1900,46 +1985,46 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C4" s="6">
         <v>36456</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="I4" s="1">
         <v>399</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1947,46 +2032,46 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6">
         <v>37360</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="I5" s="1">
         <v>100</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1994,46 +2079,46 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C6" s="6">
         <v>36370</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I6" s="1">
         <v>40</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2056,7 +2141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BED87B-A081-4D54-B5DB-8C4861187D26}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2072,41 +2157,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="A1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2114,16 +2199,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C3" s="13">
         <v>44844</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="14">
         <v>3</v>
@@ -2132,7 +2217,7 @@
         <v>89.97</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2140,16 +2225,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C4" s="25">
         <v>44844</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14">
         <v>1</v>
@@ -2158,7 +2243,7 @@
         <v>73.989999999999995</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2167,7 +2252,7 @@
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="14">
         <v>1</v>
@@ -2180,16 +2265,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C6" s="13">
         <v>44849</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="14">
         <v>10</v>
@@ -2198,7 +2283,7 @@
         <v>80</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2206,16 +2291,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C7" s="13">
         <v>44849</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="14">
         <v>2</v>
@@ -2224,7 +2309,7 @@
         <v>64</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2232,16 +2317,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C8" s="13">
         <v>44849</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F8" s="14">
         <v>4</v>
@@ -2250,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2258,16 +2343,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C9" s="13">
         <v>44850</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F9" s="14">
         <v>2</v>
@@ -2276,7 +2361,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2284,16 +2369,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C10" s="13">
         <v>44850</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
@@ -2302,7 +2387,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>